<commit_message>
refactor and update the template to freeze after shipment no
Change-Id: I15854c588efaec03d9e99f0274770ae856512914
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -400,6 +400,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -414,15 +423,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,78 +743,78 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <pane xSplit="7" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="13" style="12" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="12" style="12" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="12" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" style="12" customWidth="1"/>
-    <col min="8" max="9" width="15" style="12" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="12" customWidth="1"/>
-    <col min="11" max="11" width="33.140625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="36.28515625" style="12" customWidth="1"/>
-    <col min="13" max="14" width="15.140625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="28.85546875" style="12" customWidth="1"/>
-    <col min="16" max="16" width="30.28515625" style="12" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="12" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="12" customWidth="1"/>
-    <col min="19" max="19" width="21.28515625" style="12" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" style="12" customWidth="1"/>
-    <col min="21" max="21" width="18.140625" style="12" customWidth="1"/>
-    <col min="22" max="22" width="19.7109375" style="12" customWidth="1"/>
+    <col min="1" max="1" width="13" style="7" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" style="7" customWidth="1"/>
+    <col min="8" max="9" width="15" style="7" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" style="7" customWidth="1"/>
+    <col min="13" max="14" width="15.140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" style="7" customWidth="1"/>
+    <col min="16" max="16" width="30.28515625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="13.28515625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="7" customWidth="1"/>
+    <col min="19" max="19" width="21.28515625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" style="7" customWidth="1"/>
+    <col min="21" max="21" width="18.140625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="19.7109375" style="7" customWidth="1"/>
     <col min="23" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="63" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="9" t="s">
+      <c r="N1" s="13"/>
+      <c r="O1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="10"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="2" t="s">
         <v>29</v>
       </c>
@@ -827,20 +827,20 @@
       <c r="T1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="11"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
       <c r="I2" s="4" t="s">
         <v>56</v>
       </c>
@@ -877,51 +877,51 @@
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="R3" s="13"/>
+      <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:22">
-      <c r="R4" s="13"/>
+      <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:22">
-      <c r="R5" s="13"/>
+      <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:22">
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="R6" s="13"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:22">
-      <c r="R7" s="13"/>
+      <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="R8" s="13"/>
+      <c r="R8" s="8"/>
     </row>
     <row r="9" spans="1:22">
-      <c r="R9" s="13"/>
+      <c r="R9" s="8"/>
     </row>
     <row r="10" spans="1:22">
-      <c r="R10" s="13"/>
+      <c r="R10" s="8"/>
     </row>
     <row r="11" spans="1:22">
-      <c r="R11" s="13"/>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="R12" s="13"/>
+      <c r="R12" s="8"/>
     </row>
     <row r="13" spans="1:22">
-      <c r="R13" s="13"/>
+      <c r="R13" s="8"/>
     </row>
     <row r="14" spans="1:22">
-      <c r="R14" s="13"/>
+      <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:22">
-      <c r="R15" s="13"/>
+      <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:22">
-      <c r="R16" s="13"/>
+      <c r="R16" s="8"/>
     </row>
     <row r="17" spans="18:18">
-      <c r="R17" s="13"/>
+      <c r="R17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>